<commit_message>
R Project and Data
Created new R project and downloaded data from https://github.com/fivethirtyeight/russian-troll-tweets
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickbrowen\Documents\GitHub\SeniorProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED6A71E-02E6-4C72-ACC7-7C2384B2E329}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8DD4AFE0-063F-4A8C-BAF3-284B3CE328C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4130" xr2:uid="{38D714CD-DE5F-44FF-9BD4-A91D79505D61}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Time Worked</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Learning dplyr</t>
+  </si>
+  <si>
+    <t>Learning tidytext</t>
+  </si>
+  <si>
+    <t>Learning dplyr/ tidytext</t>
   </si>
 </sst>
 </file>
@@ -75,11 +90,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C1BFE6-A087-4A70-8C2B-05BD5EA94BB3}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,9 +423,10 @@
     <col min="1" max="1" width="11.54296875" style="2" customWidth="1"/>
     <col min="2" max="3" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -420,101 +439,221 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>43453</v>
+        <v>43430</v>
       </c>
       <c r="B2" s="1">
-        <v>0.45347222222222222</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C2" s="1">
-        <v>0.4770833333333333</v>
+        <v>0.625</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B2</f>
-        <v>2.3611111111111083E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D3" s="3" t="str">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>43454</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="D3" s="3">
         <f>IF(OR(ISBLANK(B3),ISBLANK(C3)), "", C3-B3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D4" s="3" t="str">
+        <v>5.5555555555555469E-2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>43455</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" ref="D4:D67" si="0">IF(OR(ISBLANK(B4),ISBLANK(C4)), "", C4-B4)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>43458</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="D5" s="3">
+        <f>IF(OR(ISBLANK(B5),ISBLANK(C5)), "", C5-B5)</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>43460</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>43462</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>43463</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>43469</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>43469</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>43472</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Sentiment Update - NRC Lex
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickbrowen\Documents\GitHub\SeniorProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5FB275-6C87-4F3F-8445-1D88FA058D6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD5EA22-266A-4414-89B2-FF1364ACBF27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4130" xr2:uid="{38D714CD-DE5F-44FF-9BD4-A91D79505D61}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C1BFE6-A087-4A70-8C2B-05BD5EA94BB3}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1282,10 +1282,23 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="A46" s="2">
+        <v>43516</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D47" s="3" t="str">

</xml_diff>

<commit_message>
Author and Tweet Level Analysis
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickbrowen\Documents\GitHub\SeniorProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD5EA22-266A-4414-89B2-FF1364ACBF27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFD85CB-441F-44B5-8707-F687F546EDD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4130" xr2:uid="{38D714CD-DE5F-44FF-9BD4-A91D79505D61}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Git issues</t>
+  </si>
+  <si>
+    <t>Author Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author Analysis </t>
   </si>
 </sst>
 </file>
@@ -440,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C1BFE6-A087-4A70-8C2B-05BD5EA94BB3}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,108 +1307,205 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="A47" s="2">
+        <v>43517</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>43517</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>43523</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D49" s="3">
+        <f>IF(OR(ISBLANK(B49),ISBLANK(C49)), "", C49-B49)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>43524</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>43524</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>43525</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>43526</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>43528</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D55" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D56" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D57" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D58" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D61" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D62" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D63" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D64" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>